<commit_message>
Add 1 to l1,5 prefetch feature
</commit_message>
<xml_diff>
--- a/DOC/CLUSTER_ICACHE_CTRL_reference.xlsx
+++ b/DOC/CLUSTER_ICACHE_CTRL_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -36,69 +36,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="148">
-  <si>
-    <t>Document Information</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>FC_ICACHE_CTRL reference</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>IP reference</t>
-  </si>
-  <si>
-    <t>Author</t>
-  </si>
-  <si>
-    <t>Florent Rotenberg</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Fisrt Release</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>FC_ICACHE_CTRL interface definition</t>
-  </si>
-  <si>
-    <t>IP Information</t>
-  </si>
-  <si>
-    <t>IP type</t>
-  </si>
-  <si>
-    <t>FC_ICACHE_CTRL</t>
-  </si>
-  <si>
-    <t>Delivery Type</t>
-  </si>
-  <si>
-    <t>History</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Modification</t>
-  </si>
-  <si>
-    <t>26/10/2016</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="158">
+  <si>
+    <t xml:space="preserve">Document Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC_ICACHE_CTRL reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florent Rotenberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fisrt Release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC_ICACHE_CTRL interface definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FC_ICACHE_CTRL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">History</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/10/2016</t>
   </si>
   <si>
     <r>
@@ -109,7 +109,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>1</t>
+      <t xml:space="preserve">1</t>
     </r>
     <r>
       <rPr>
@@ -120,7 +120,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>st</t>
+      <t xml:space="preserve">st</t>
     </r>
     <r>
       <rPr>
@@ -130,390 +130,519 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> release</t>
+      <t xml:space="preserve"> release</t>
     </r>
   </si>
   <si>
-    <t>F.Rotenberg</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>This sheet. General information about document usage</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Guidelines on how to used the various sheet</t>
-  </si>
-  <si>
-    <t>IP Release</t>
-  </si>
-  <si>
-    <t>Release information sheet describing</t>
-  </si>
-  <si>
-    <t>IPIF_relx.x</t>
-  </si>
-  <si>
-    <t>IP interface description reference, describing IP symbol/entity and integration and test information relative to IP interface.</t>
-  </si>
-  <si>
-    <t>IPDESCR_Relx.x</t>
-  </si>
-  <si>
-    <t>Description of the main features of the IP</t>
-  </si>
-  <si>
-    <t>IPREGLIST_rely.y</t>
-  </si>
-  <si>
-    <t>Description of the list of registers used by IP. Registers can be physically instanciated inside IP or outside IP.</t>
-  </si>
-  <si>
-    <t>IPREGMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of bit fields when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
-  </si>
-  <si>
-    <t>IPTREGMAP_relz.z</t>
-  </si>
-  <si>
-    <t>Description of mapping of test bit field when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
-  </si>
-  <si>
-    <t>IP Release Sheet</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Possible Value</t>
-  </si>
-  <si>
-    <t>IP release version numeroted as [major release].[minor release]. A release is major whenever IP interface is modified.</t>
-  </si>
-  <si>
-    <t>X.Y. Z</t>
-  </si>
-  <si>
-    <t>Release description</t>
-  </si>
-  <si>
-    <t>This is a free text entry expliciting the release main modifications and purpose.</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>IPIF</t>
-  </si>
-  <si>
-    <t>IPIF sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPDESCR</t>
-  </si>
-  <si>
-    <t>IPDESCR sheet version to nbe used for this release</t>
-  </si>
-  <si>
-    <t>X.Y.Z</t>
-  </si>
-  <si>
-    <t>IPREGLIST</t>
-  </si>
-  <si>
-    <t>IPREGLIST sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPREGMAP</t>
-  </si>
-  <si>
-    <t>IPREGMAP sheet version to be used for this release.</t>
-  </si>
-  <si>
-    <t>IPDOC</t>
-  </si>
-  <si>
-    <t>IPDOC version to be used for this release.</t>
-  </si>
-  <si>
-    <t>GIT version</t>
-  </si>
-  <si>
-    <t>GIT database number corresponding to IP design code and IP reference XLS.</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>IPIF sheet</t>
-  </si>
-  <si>
-    <t>IP Interface description</t>
-  </si>
-  <si>
-    <t>IP Pin Name</t>
-  </si>
-  <si>
-    <t>Name of IP Pin. This must must exactly name find in code or schematic (including case).</t>
-  </si>
-  <si>
-    <t>Direction</t>
-  </si>
-  <si>
-    <t>Direction or type of signal</t>
-  </si>
-  <si>
-    <t>In,Out,IO</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Analog, Digital, supply, DR (Dual Rail), SR (SingleRail)</t>
-  </si>
-  <si>
-    <t>Analog,Digital, VDD, GND, DR, SR</t>
-  </si>
-  <si>
-    <t>Voltage Domain</t>
-  </si>
-  <si>
-    <t>Clock domain</t>
-  </si>
-  <si>
-    <t>IO</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Reset Value</t>
-  </si>
-  <si>
-    <t>Integration information</t>
-  </si>
-  <si>
-    <t>Integration comment</t>
-  </si>
-  <si>
-    <t>Core Interface</t>
-  </si>
-  <si>
-    <t>Register  Interface</t>
-  </si>
-  <si>
-    <t>Register name</t>
-  </si>
-  <si>
-    <t>DFT value</t>
-  </si>
-  <si>
-    <t>Level Shifter</t>
-  </si>
-  <si>
-    <t>Isolation cell</t>
-  </si>
-  <si>
-    <t>Connected to</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>Drive</t>
-  </si>
-  <si>
-    <t>Destination supply</t>
-  </si>
-  <si>
-    <t>Hard Macro information</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>Antenna</t>
-  </si>
-  <si>
-    <t>Additonal Information</t>
-  </si>
-  <si>
-    <t>FreeText 1</t>
-  </si>
-  <si>
-    <t>FreeText 2</t>
-  </si>
-  <si>
-    <t>Driver information</t>
-  </si>
-  <si>
-    <t>Function1</t>
-  </si>
-  <si>
-    <t>Function2</t>
-  </si>
-  <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
-    <t>Rel1.0.0</t>
-  </si>
-  <si>
-    <t>Bit position</t>
-  </si>
-  <si>
-    <t>Trim during production</t>
-  </si>
-  <si>
-    <t>clk_i</t>
-  </si>
-  <si>
-    <t>IN</t>
-  </si>
-  <si>
-    <t>digital</t>
-  </si>
-  <si>
-    <t>rstn_i</t>
-  </si>
-  <si>
-    <t>CL_ICACHE_CTRL component manages the following features:
+    <t xml:space="preserve">F.Rotenberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sheet. General information about document usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guidelines on how to used the various sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release information sheet describing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF_relx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP interface description reference, describing IP symbol/entity and integration and test information relative to IP interface.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR_Relx.x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the main features of the IP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST_rely.y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of the list of registers used by IP. Registers can be physically instanciated inside IP or outside IP.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of bit fields when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPTREGMAP_relz.z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description of mapping of test bit field when registers are internal to IP. This sheet is optional for IP which are not instanciating registers as information can be build from IPIF and IPRELIST sheet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Release Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP release version numeroted as [major release].[minor release]. A release is major whenever IP interface is modified.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X.Y. Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Release description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a free text entry expliciting the release main modifications and purpose.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDESCR sheet version to nbe used for this release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X.Y.Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGLIST sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPREGMAP sheet version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPDOC version to be used for this release.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GIT database number corresponding to IP design code and IP reference XLS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPIF sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Interface description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP Pin Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of IP Pin. This must must exactly name find in code or schematic (including case).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction or type of signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In,Out,IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog, Digital, supply, DR (Dual Rail), SR (SingleRail)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analog,Digital, VDD, GND, DR, SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register  Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFT value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level Shifter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolation cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connected to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard Macro information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additonal Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rel1.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trim during production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rstn_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL_ICACHE_CTRL component manages the following features:
 - Bypassable Cluster instruction cache controller
 - Flush and selective flush commands</t>
   </si>
   <si>
-    <t>Register Name</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Register Type</t>
-  </si>
-  <si>
-    <t>Host Access Type</t>
-  </si>
-  <si>
-    <t>IP access Type</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>FootNote</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Hide</t>
-  </si>
-  <si>
-    <t>ENABLE</t>
-  </si>
-  <si>
-    <t>0x0</t>
-  </si>
-  <si>
-    <t>Config</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Cluster instruction cache unit enable configuration register.</t>
-  </si>
-  <si>
-    <t>FLUSH</t>
-  </si>
-  <si>
-    <t>0x4</t>
-  </si>
-  <si>
-    <t>Cluster instruction cache unit flush command register.</t>
-  </si>
-  <si>
-    <t>L0_FLUSH</t>
-  </si>
-  <si>
-    <t>0x8</t>
-  </si>
-  <si>
-    <t>Cluster level 0 instruction cache unit flush command register.</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>SEL_FLUSH</t>
-  </si>
-  <si>
-    <t>0xC</t>
-  </si>
-  <si>
-    <t>Cluster instruction cache unit selective flush command register.</t>
-  </si>
-  <si>
-    <t>IS_PRIVATE</t>
-  </si>
-  <si>
-    <t>0x10</t>
-  </si>
-  <si>
-    <t>Bit field</t>
-  </si>
-  <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>Bit Position</t>
-  </si>
-  <si>
-    <t>EN</t>
-  </si>
-  <si>
-    <t>Cluster instruction cache enable configuration bitfield:
+    <t xml:space="preserve">Register Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host Access Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP access Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FootNote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction cache unit enable configuration register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLUSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction cache unit flush command register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L0_FLUSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster level 0 instruction cache unit flush command register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEL_FLUSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction cache unit selective flush command register.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENABLE_SPECIAL_CORE_CACHE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x18</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">When use 9</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> core, the number 8 core can have seperated icache or its own icache. Use this register to control.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ENABLE_L1_L15_PREFETCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x1C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For each Level 0 private cache, enable L0 to L0.5, (also called L1 to L1.5) prefetch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bit Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN_PRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction private cache enable configuration bitfield:
 - 1'b0: disabled
 - 1'b1: enabled</t>
   </si>
   <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>Cluster instruction cache full flush command.</t>
-  </si>
-  <si>
-    <t>L0_FL</t>
-  </si>
-  <si>
-    <t>Cluster level 0 instruction cache full flush command. </t>
-  </si>
-  <si>
-    <t>ADDR</t>
-  </si>
-  <si>
-    <t>Cluster instruction cache selective flush address configuration bitfield.</t>
-  </si>
-  <si>
-    <t>testcase location&amp;name</t>
+    <t xml:space="preserve">EN_SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction shared cache banks enable configuration bitfield:
+- 1'b0: disabled
+- 1'b1: enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FL_PRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction private cache full flush command.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FL_SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction shared cache banks full flush command.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L0_FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster level 0 instruction cache full flush command. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cluster instruction cache selective flush address configuration bitfield.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Enable or disable 9</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> core seperated icache:
+- 1'b0: disabled
+- 1'b1: enabled</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Enable or disable all 9</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> private icache prefetch feature, for each bitfield:
+- 9'b000000000: disabled all private icache prefetch
+- 9'b000000001: enabled private icache 0 prefetch
+- 9'b000000011: enabled private icache 0, 1  prefetch
+...
+- 9'b111111111: enabled all private icache prefetch</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">testcase location&amp;name</t>
   </si>
 </sst>
 </file>
@@ -521,7 +650,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -718,7 +847,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -957,6 +1086,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1043,16 +1176,16 @@
   </sheetPr>
   <dimension ref="B1:D29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,7 +1424,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1306,17 +1439,17 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="9.71938775510204"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="1" width="9.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,7 +1780,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1662,17 +1795,17 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.71938775510204"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="42.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="9.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,7 +1854,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1736,22 +1869,22 @@
   </sheetPr>
   <dimension ref="A1:AMC5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="2" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1017" min="23" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="8.10204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="23" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="8.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +3099,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2981,14 +3114,14 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="52" width="171.709183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="52" width="171.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,7 +3137,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3017,29 +3150,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="5.66836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="46.7091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="54" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.10204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="54" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="8.1"/>
   </cols>
   <sheetData>
     <row r="1" s="56" customFormat="true" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,7 +3267,7 @@
       </c>
       <c r="J3" s="57"/>
     </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="57" t="s">
         <v>127</v>
       </c>
@@ -3190,7 +3323,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
         <v>134</v>
       </c>
@@ -3212,9 +3345,37 @@
       <c r="H6" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="I6" s="56"/>
+      <c r="I6" s="56" t="s">
+        <v>136</v>
+      </c>
       <c r="L6" s="54" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="56" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3226,7 +3387,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3239,37 +3400,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="71.4081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="54" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.10204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="71.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="54" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="42" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>75</v>
@@ -3290,9 +3451,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="57" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B2" s="57" t="s">
         <v>118</v>
@@ -3301,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="52" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E2" s="56" t="s">
         <v>121</v>
@@ -3313,21 +3474,21 @@
         <v>119</v>
       </c>
       <c r="H2" s="59" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="57" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C3" s="52" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D3" s="52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="56" t="s">
         <v>121</v>
@@ -3339,21 +3500,21 @@
         <v>119</v>
       </c>
       <c r="H3" s="59" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="57" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C4" s="52" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="52" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E4" s="56" t="s">
         <v>121</v>
@@ -3365,24 +3526,21 @@
         <v>119</v>
       </c>
       <c r="H4" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="I4" s="54" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="43" t="n">
-        <v>32</v>
+      <c r="A5" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="52" t="n">
+        <v>9</v>
+      </c>
+      <c r="D5" s="52" t="n">
+        <v>2</v>
       </c>
       <c r="E5" s="56" t="s">
         <v>121</v>
@@ -3390,19 +3548,127 @@
       <c r="F5" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="58" t="s">
         <v>119</v>
       </c>
       <c r="H5" s="59" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="52" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="I6" s="54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="43" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="65.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="54" t="n">
+        <v>9</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3417,36 +3683,36 @@
   </sheetPr>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="75.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="60" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="60" t="s">
+      <c r="C1" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>